<commit_message>
Updated not deterministic graphs
</commit_message>
<xml_diff>
--- a/Graphs/H2.xlsx
+++ b/Graphs/H2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tasmiashahriar/Desktop/CSC 722/Project/EvalDQNsOffline/Graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C655FF3-25CE-FE44-AA54-74783318F5AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB75F60-B96A-D54C-BEBA-1FA77701B2F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="560" windowWidth="26440" windowHeight="13980" activeTab="2" xr2:uid="{9E95AFC6-744F-814A-B055-638CB44968AC}"/>
+    <workbookView xWindow="2360" yWindow="560" windowWidth="26440" windowHeight="13980" activeTab="1" xr2:uid="{9E95AFC6-744F-814A-B055-638CB44968AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Gridworld_dm" sheetId="1" r:id="rId1"/>
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98436158-DF1E-0141-B577-72D2B20F6A79}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,7 +833,7 @@
         <v>1000</v>
       </c>
       <c r="D2">
-        <v>-0.5</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -847,7 +847,7 @@
         <v>1000</v>
       </c>
       <c r="D3">
-        <v>9.5</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -861,7 +861,7 @@
         <v>1000</v>
       </c>
       <c r="D4">
-        <v>3.1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -875,7 +875,7 @@
         <v>1000</v>
       </c>
       <c r="D5">
-        <v>3.7</v>
+        <v>20.100000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -889,7 +889,7 @@
         <v>1000</v>
       </c>
       <c r="D6">
-        <v>-0.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -903,7 +903,7 @@
         <v>1000</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>25.8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -917,7 +917,7 @@
         <v>1000</v>
       </c>
       <c r="D8">
-        <v>-0.8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -931,7 +931,7 @@
         <v>1000</v>
       </c>
       <c r="D9">
-        <v>7.6</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -945,7 +945,7 @@
         <v>5000</v>
       </c>
       <c r="D10">
-        <v>3.8</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -959,7 +959,7 @@
         <v>5000</v>
       </c>
       <c r="D11">
-        <v>1.8</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -973,7 +973,7 @@
         <v>5000</v>
       </c>
       <c r="D12">
-        <v>-0.6</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -987,7 +987,7 @@
         <v>5000</v>
       </c>
       <c r="D13">
-        <v>3.8</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1001,7 +1001,7 @@
         <v>5000</v>
       </c>
       <c r="D14">
-        <v>3.8</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1015,7 +1015,7 @@
         <v>5000</v>
       </c>
       <c r="D15">
-        <v>-1.2</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1029,7 +1029,7 @@
         <v>5000</v>
       </c>
       <c r="D16">
-        <v>5.7</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1043,7 +1043,7 @@
         <v>5000</v>
       </c>
       <c r="D17">
-        <v>0.5</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1057,7 +1057,7 @@
         <v>10000</v>
       </c>
       <c r="D18">
-        <v>6.6</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1071,7 +1071,7 @@
         <v>10000</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1085,7 +1085,7 @@
         <v>10000</v>
       </c>
       <c r="D20">
-        <v>3.3</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1099,7 +1099,7 @@
         <v>10000</v>
       </c>
       <c r="D21">
-        <v>-0.5</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1113,7 +1113,7 @@
         <v>10000</v>
       </c>
       <c r="D22">
-        <v>6.6</v>
+        <v>5.4</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1128,7 +1128,7 @@
         <v>10000</v>
       </c>
       <c r="D23">
-        <v>4.9000000000000004</v>
+        <v>12.7</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1143,7 +1143,7 @@
         <v>10000</v>
       </c>
       <c r="D24">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1219,7 +1219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA3E9DB-CF56-7F45-9F44-86B6DFEB0BB7}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>

</xml_diff>